<commit_message>
running script including 2017 data
</commit_message>
<xml_diff>
--- a/information/raw_databases/SERNAPESCA/landings/landings_artisanal_per_species_region_2017.xlsx
+++ b/information/raw_databases/SERNAPESCA/landings/landings_artisanal_per_species_region_2017.xlsx
@@ -1,19 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargaspoulsen/github/main-fisheries-chile/information/raw_databases/SERNAPESCA/landings/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19440" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="19440" windowHeight="12340"/>
   </bookViews>
   <sheets>
-    <sheet name="des_art_región" sheetId="1" r:id="rId1"/>
+    <sheet name="des_art_region" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">des_art_región!$A$5:$P$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">des_art_región!$1:$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">des_art_region!$A$5:$P$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">des_art_region!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -615,10 +628,10 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,7 +640,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,12 +768,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -790,12 +803,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -999,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q161"/>
@@ -1008,14 +1021,14 @@
       <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>151</v>
       </c>
@@ -1035,7 +1048,7 @@
       <c r="O1" s="20"/>
       <c r="P1" s="20"/>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
@@ -1055,7 +1068,7 @@
       <c r="O2" s="20"/>
       <c r="P2" s="20"/>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -1075,7 +1088,7 @@
       <c r="O3" s="20"/>
       <c r="P3" s="20"/>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1092,7 +1105,7 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" s="4" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
         <v>157</v>
       </c>
@@ -1193,7 +1206,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
         <v>152</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1308,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
@@ -1346,7 +1359,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -1397,7 +1410,7 @@
         <v>9724</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1461,7 @@
         <v>29897</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
         <v>158</v>
       </c>
@@ -1499,7 +1512,7 @@
         <v>211257</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
@@ -1550,7 +1563,7 @@
         <v>71771</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1601,7 +1614,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>24</v>
       </c>
@@ -1652,7 +1665,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
@@ -1703,7 +1716,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
@@ -1754,7 +1767,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
@@ -1805,7 +1818,7 @@
         <v>21267</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
@@ -1856,7 +1869,7 @@
         <v>20012</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
         <v>29</v>
       </c>
@@ -1907,7 +1920,7 @@
         <v>47584</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -1925,7 +1938,7 @@
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
@@ -1976,7 +1989,7 @@
         <v>5337</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
         <v>31</v>
       </c>
@@ -2027,7 +2040,7 @@
         <v>234268</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="10" t="s">
         <v>32</v>
       </c>
@@ -2078,7 +2091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="10" t="s">
         <v>33</v>
       </c>
@@ -2129,7 +2142,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="10" t="s">
         <v>34</v>
       </c>
@@ -2180,7 +2193,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>35</v>
       </c>
@@ -2231,7 +2244,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="10" t="s">
         <v>36</v>
       </c>
@@ -2282,7 +2295,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="10" t="s">
         <v>146</v>
       </c>
@@ -2333,7 +2346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="10" t="s">
         <v>37</v>
       </c>
@@ -2384,7 +2397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="10" t="s">
         <v>38</v>
       </c>
@@ -2435,7 +2448,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="10" t="s">
         <v>39</v>
       </c>
@@ -2486,7 +2499,7 @@
         <v>59982</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="10" t="s">
         <v>159</v>
       </c>
@@ -2537,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="10" t="s">
         <v>40</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="10" t="s">
         <v>41</v>
       </c>
@@ -2639,7 +2652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="10" t="s">
         <v>160</v>
       </c>
@@ -2690,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="10" t="s">
         <v>42</v>
       </c>
@@ -2741,7 +2754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="10" t="s">
         <v>43</v>
       </c>
@@ -2792,7 +2805,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="10" t="s">
         <v>147</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="10" t="s">
         <v>44</v>
       </c>
@@ -2894,7 +2907,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="10" t="s">
         <v>45</v>
       </c>
@@ -2945,7 +2958,7 @@
         <v>22013</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="10" t="s">
         <v>46</v>
       </c>
@@ -2996,7 +3009,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="10" t="s">
         <v>47</v>
       </c>
@@ -3047,7 +3060,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="10" t="s">
         <v>48</v>
       </c>
@@ -3098,7 +3111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="10" t="s">
         <v>153</v>
       </c>
@@ -3149,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="10" t="s">
         <v>49</v>
       </c>
@@ -3200,7 +3213,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="10" t="s">
         <v>50</v>
       </c>
@@ -3251,7 +3264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="10" t="s">
         <v>51</v>
       </c>
@@ -3302,7 +3315,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="49" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="10" t="s">
         <v>52</v>
       </c>
@@ -3353,7 +3366,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="50" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="10" t="s">
         <v>53</v>
       </c>
@@ -3404,7 +3417,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="51" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="10" t="s">
         <v>54</v>
       </c>
@@ -3455,7 +3468,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="52" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="10" t="s">
         <v>148</v>
       </c>
@@ -3506,7 +3519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="10" t="s">
         <v>55</v>
       </c>
@@ -3557,7 +3570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="10" t="s">
         <v>56</v>
       </c>
@@ -3608,7 +3621,7 @@
         <v>29413</v>
       </c>
     </row>
-    <row r="55" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="10" t="s">
         <v>57</v>
       </c>
@@ -3659,7 +3672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="10" t="s">
         <v>154</v>
       </c>
@@ -3710,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="10" t="s">
         <v>58</v>
       </c>
@@ -3761,7 +3774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="10" t="s">
         <v>59</v>
       </c>
@@ -3812,7 +3825,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="10" t="s">
         <v>60</v>
       </c>
@@ -3863,7 +3876,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="10" t="s">
         <v>61</v>
       </c>
@@ -3914,7 +3927,7 @@
         <v>29954</v>
       </c>
     </row>
-    <row r="61" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="10" t="s">
         <v>62</v>
       </c>
@@ -3965,7 +3978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="10" t="s">
         <v>63</v>
       </c>
@@ -4016,7 +4029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="10" t="s">
         <v>161</v>
       </c>
@@ -4067,7 +4080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="10" t="s">
         <v>64</v>
       </c>
@@ -4118,7 +4131,7 @@
         <v>7748</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="10" t="s">
         <v>65</v>
       </c>
@@ -4169,7 +4182,7 @@
         <v>5375</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="10" t="s">
         <v>149</v>
       </c>
@@ -4220,7 +4233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="10" t="s">
         <v>162</v>
       </c>
@@ -4271,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="10" t="s">
         <v>66</v>
       </c>
@@ -4322,7 +4335,7 @@
         <v>22959</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="10" t="s">
         <v>150</v>
       </c>
@@ -4373,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="10" t="s">
         <v>67</v>
       </c>
@@ -4424,7 +4437,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="71" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="10" t="s">
         <v>68</v>
       </c>
@@ -4475,7 +4488,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="10" t="s">
         <v>69</v>
       </c>
@@ -4526,7 +4539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="10" t="s">
         <v>70</v>
       </c>
@@ -4577,7 +4590,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="10" t="s">
         <v>71</v>
       </c>
@@ -4628,7 +4641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="10" t="s">
         <v>163</v>
       </c>
@@ -4679,7 +4692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="10" t="s">
         <v>72</v>
       </c>
@@ -4730,7 +4743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="10" t="s">
         <v>73</v>
       </c>
@@ -4781,7 +4794,7 @@
         <v>22485</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="10" t="s">
         <v>74</v>
       </c>
@@ -4832,7 +4845,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="10" t="s">
         <v>75</v>
       </c>
@@ -4883,7 +4896,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="10" t="s">
         <v>76</v>
       </c>
@@ -4934,7 +4947,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="10" t="s">
         <v>77</v>
       </c>
@@ -4985,7 +4998,7 @@
         <v>19293</v>
       </c>
     </row>
-    <row r="82" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="10" t="s">
         <v>78</v>
       </c>
@@ -5036,7 +5049,7 @@
         <v>321589</v>
       </c>
     </row>
-    <row r="83" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="10" t="s">
         <v>79</v>
       </c>
@@ -5087,7 +5100,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="84" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="10" t="s">
         <v>80</v>
       </c>
@@ -5138,7 +5151,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="10" t="s">
         <v>81</v>
       </c>
@@ -5189,7 +5202,7 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="86" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="10" t="s">
         <v>164</v>
       </c>
@@ -5240,7 +5253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="10" t="s">
         <v>165</v>
       </c>
@@ -5291,7 +5304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="10" t="s">
         <v>82</v>
       </c>
@@ -5342,7 +5355,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="89" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="10" t="s">
         <v>83</v>
       </c>
@@ -5393,7 +5406,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="90" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="10" t="s">
         <v>84</v>
       </c>
@@ -5444,7 +5457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="10" t="s">
         <v>85</v>
       </c>
@@ -5495,7 +5508,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="92" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="12" t="s">
         <v>86</v>
       </c>
@@ -5546,7 +5559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="10"/>
       <c r="B93" s="11"/>
       <c r="C93" s="11"/>
@@ -5564,7 +5577,7 @@
       <c r="O93" s="11"/>
       <c r="P93" s="11"/>
     </row>
-    <row r="94" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
         <v>87</v>
       </c>
@@ -5615,7 +5628,7 @@
         <v>15672</v>
       </c>
     </row>
-    <row r="95" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="10" t="s">
         <v>155</v>
       </c>
@@ -5666,7 +5679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="10" t="s">
         <v>88</v>
       </c>
@@ -5717,7 +5730,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="97" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="10" t="s">
         <v>89</v>
       </c>
@@ -5768,7 +5781,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="98" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="10" t="s">
         <v>90</v>
       </c>
@@ -5819,7 +5832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="10" t="s">
         <v>156</v>
       </c>
@@ -5870,7 +5883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="10" t="s">
         <v>91</v>
       </c>
@@ -5921,7 +5934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="10" t="s">
         <v>92</v>
       </c>
@@ -5972,7 +5985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="102" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="10" t="s">
         <v>93</v>
       </c>
@@ -6023,7 +6036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="10" t="s">
         <v>94</v>
       </c>
@@ -6074,7 +6087,7 @@
         <v>7031</v>
       </c>
     </row>
-    <row r="104" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="10" t="s">
         <v>95</v>
       </c>
@@ -6125,7 +6138,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="105" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="10" t="s">
         <v>96</v>
       </c>
@@ -6176,7 +6189,7 @@
         <v>2374</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="10" t="s">
         <v>97</v>
       </c>
@@ -6227,7 +6240,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="107" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="10" t="s">
         <v>98</v>
       </c>
@@ -6278,7 +6291,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="108" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="10" t="s">
         <v>99</v>
       </c>
@@ -6329,7 +6342,7 @@
         <v>113405</v>
       </c>
     </row>
-    <row r="109" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="10" t="s">
         <v>100</v>
       </c>
@@ -6380,7 +6393,7 @@
         <v>4186</v>
       </c>
     </row>
-    <row r="110" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="10" t="s">
         <v>101</v>
       </c>
@@ -6431,7 +6444,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="10" t="s">
         <v>102</v>
       </c>
@@ -6482,7 +6495,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="112" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="10" t="s">
         <v>103</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="10" t="s">
         <v>104</v>
       </c>
@@ -6584,7 +6597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="10" t="s">
         <v>105</v>
       </c>
@@ -6635,7 +6648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="10" t="s">
         <v>106</v>
       </c>
@@ -6686,7 +6699,7 @@
         <v>2717</v>
       </c>
     </row>
-    <row r="116" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="10" t="s">
         <v>107</v>
       </c>
@@ -6737,7 +6750,7 @@
         <v>2718</v>
       </c>
     </row>
-    <row r="117" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="10" t="s">
         <v>108</v>
       </c>
@@ -6788,7 +6801,7 @@
         <v>5983</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="10" t="s">
         <v>109</v>
       </c>
@@ -6839,7 +6852,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="119" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="10" t="s">
         <v>110</v>
       </c>
@@ -6890,7 +6903,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="10" t="s">
         <v>111</v>
       </c>
@@ -6941,7 +6954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="10" t="s">
         <v>112</v>
       </c>
@@ -6992,7 +7005,7 @@
         <v>2864</v>
       </c>
     </row>
-    <row r="122" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="10" t="s">
         <v>113</v>
       </c>
@@ -7043,7 +7056,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="123" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="10" t="s">
         <v>114</v>
       </c>
@@ -7094,7 +7107,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="124" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="12" t="s">
         <v>115</v>
       </c>
@@ -7145,7 +7158,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="125" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="10"/>
       <c r="B125" s="11"/>
       <c r="C125" s="11"/>
@@ -7163,7 +7176,7 @@
       <c r="O125" s="11"/>
       <c r="P125" s="11"/>
     </row>
-    <row r="126" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="10" t="s">
         <v>116</v>
       </c>
@@ -7214,7 +7227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="10" t="s">
         <v>117</v>
       </c>
@@ -7265,7 +7278,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="128" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="10" t="s">
         <v>118</v>
       </c>
@@ -7316,7 +7329,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="129" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="10" t="s">
         <v>119</v>
       </c>
@@ -7367,7 +7380,7 @@
         <v>5017</v>
       </c>
     </row>
-    <row r="130" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="10" t="s">
         <v>120</v>
       </c>
@@ -7418,7 +7431,7 @@
         <v>6138</v>
       </c>
     </row>
-    <row r="131" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="10" t="s">
         <v>121</v>
       </c>
@@ -7469,7 +7482,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="132" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="10" t="s">
         <v>122</v>
       </c>
@@ -7520,7 +7533,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="133" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="10" t="s">
         <v>123</v>
       </c>
@@ -7571,7 +7584,7 @@
         <v>4874</v>
       </c>
     </row>
-    <row r="134" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="10" t="s">
         <v>124</v>
       </c>
@@ -7622,7 +7635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="135" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="10" t="s">
         <v>125</v>
       </c>
@@ -7673,7 +7686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="10" t="s">
         <v>126</v>
       </c>
@@ -7724,7 +7737,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="10" t="s">
         <v>166</v>
       </c>
@@ -7775,7 +7788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="10" t="s">
         <v>127</v>
       </c>
@@ -7826,7 +7839,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="139" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="10" t="s">
         <v>128</v>
       </c>
@@ -7877,7 +7890,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="140" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="10" t="s">
         <v>129</v>
       </c>
@@ -7928,7 +7941,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="10" t="s">
         <v>130</v>
       </c>
@@ -7979,7 +7992,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="142" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="10" t="s">
         <v>131</v>
       </c>
@@ -8030,7 +8043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="143" spans="1:16" s="4" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" s="4" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="10" t="s">
         <v>132</v>
       </c>
@@ -8081,7 +8094,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="10" t="s">
         <v>133</v>
       </c>
@@ -8132,7 +8145,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="145" spans="1:17" s="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:17" s="7" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="10" t="s">
         <v>167</v>
       </c>
@@ -8183,7 +8196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="146" spans="1:17" s="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:17" s="7" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="10" t="s">
         <v>134</v>
       </c>
@@ -8234,7 +8247,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="147" spans="1:17" s="17" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:17" s="17" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="10" t="s">
         <v>135</v>
       </c>
@@ -8285,7 +8298,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="148" spans="1:17" s="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:17" s="7" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="12" t="s">
         <v>136</v>
       </c>
@@ -8336,7 +8349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:17" s="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:17" s="7" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="10"/>
       <c r="B149" s="11"/>
       <c r="C149" s="11"/>
@@ -8354,7 +8367,7 @@
       <c r="O149" s="11"/>
       <c r="P149" s="11"/>
     </row>
-    <row r="150" spans="1:17" s="7" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:17" s="7" customFormat="1" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="10" t="s">
         <v>137</v>
       </c>
@@ -8405,7 +8418,7 @@
         <v>30108</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="10" t="s">
         <v>168</v>
       </c>
@@ -8456,7 +8469,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="10" t="s">
         <v>138</v>
       </c>
@@ -8507,7 +8520,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="12" t="s">
         <v>139</v>
       </c>
@@ -8563,63 +8576,63 @@
         <v>140</v>
       </c>
       <c r="B155" s="16">
-        <f>SUM(B6:B20)</f>
+        <f t="shared" ref="B155:P155" si="4">SUM(B6:B20)</f>
         <v>215</v>
       </c>
       <c r="C155" s="16">
-        <f>SUM(C6:C20)</f>
+        <f t="shared" si="4"/>
         <v>16842</v>
       </c>
       <c r="D155" s="16">
-        <f>SUM(D6:D20)</f>
+        <f t="shared" si="4"/>
         <v>62019</v>
       </c>
       <c r="E155" s="16">
-        <f>SUM(E6:E20)</f>
+        <f t="shared" si="4"/>
         <v>116769</v>
       </c>
       <c r="F155" s="16">
-        <f>SUM(F6:F20)</f>
+        <f t="shared" si="4"/>
         <v>86685</v>
       </c>
       <c r="G155" s="16">
-        <f>SUM(G6:G20)</f>
+        <f t="shared" si="4"/>
         <v>13514</v>
       </c>
       <c r="H155" s="16">
-        <f>SUM(H6:H20)</f>
+        <f t="shared" si="4"/>
         <v>3760</v>
       </c>
       <c r="I155" s="16">
-        <f>SUM(I6:I20)</f>
+        <f t="shared" si="4"/>
         <v>2038</v>
       </c>
       <c r="J155" s="16">
-        <f>SUM(J6:J20)</f>
+        <f t="shared" si="4"/>
         <v>15808</v>
       </c>
       <c r="K155" s="16">
-        <f>SUM(K6:K20)</f>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="L155" s="16">
-        <f>SUM(L6:L20)</f>
+        <f t="shared" si="4"/>
         <v>2105</v>
       </c>
       <c r="M155" s="16">
-        <f>SUM(M6:M20)</f>
+        <f t="shared" si="4"/>
         <v>85378</v>
       </c>
       <c r="N155" s="16">
-        <f>SUM(N6:N20)</f>
+        <f t="shared" si="4"/>
         <v>1941</v>
       </c>
       <c r="O155" s="16">
-        <f>SUM(O6:O20)</f>
+        <f t="shared" si="4"/>
         <v>8346</v>
       </c>
       <c r="P155" s="16">
-        <f>SUM(P6:P20)</f>
+        <f t="shared" si="4"/>
         <v>415463</v>
       </c>
       <c r="Q155" s="5"/>
@@ -8629,63 +8642,63 @@
         <v>141</v>
       </c>
       <c r="B156" s="16">
-        <f>SUM(B22:B92)</f>
+        <f t="shared" ref="B156:P156" si="5">SUM(B22:B92)</f>
         <v>90868</v>
       </c>
       <c r="C156" s="16">
-        <f>SUM(C22:C92)</f>
+        <f t="shared" si="5"/>
         <v>19140</v>
       </c>
       <c r="D156" s="16">
-        <f>SUM(D22:D92)</f>
+        <f t="shared" si="5"/>
         <v>56032</v>
       </c>
       <c r="E156" s="16">
-        <f>SUM(E22:E92)</f>
+        <f t="shared" si="5"/>
         <v>36522</v>
       </c>
       <c r="F156" s="16">
-        <f>SUM(F22:F92)</f>
+        <f t="shared" si="5"/>
         <v>26312</v>
       </c>
       <c r="G156" s="16">
-        <f>SUM(G22:G92)</f>
+        <f t="shared" si="5"/>
         <v>11628</v>
       </c>
       <c r="H156" s="16">
-        <f>SUM(H22:H92)</f>
+        <f t="shared" si="5"/>
         <v>373</v>
       </c>
       <c r="I156" s="16">
-        <f>SUM(I22:I92)</f>
+        <f t="shared" si="5"/>
         <v>5202</v>
       </c>
       <c r="J156" s="16">
-        <f>SUM(J22:J92)</f>
+        <f t="shared" si="5"/>
         <v>434648</v>
       </c>
       <c r="K156" s="16">
-        <f>SUM(K22:K92)</f>
+        <f t="shared" si="5"/>
         <v>1531</v>
       </c>
       <c r="L156" s="16">
-        <f>SUM(L22:L92)</f>
+        <f t="shared" si="5"/>
         <v>68762</v>
       </c>
       <c r="M156" s="16">
-        <f>SUM(M22:M92)</f>
+        <f t="shared" si="5"/>
         <v>34009</v>
       </c>
       <c r="N156" s="16">
-        <f>SUM(N22:N92)</f>
+        <f t="shared" si="5"/>
         <v>6208</v>
       </c>
       <c r="O156" s="16">
-        <f>SUM(O22:O92)</f>
+        <f t="shared" si="5"/>
         <v>207</v>
       </c>
       <c r="P156" s="16">
-        <f>SUM(P22:P92)</f>
+        <f t="shared" si="5"/>
         <v>791442</v>
       </c>
       <c r="Q156" s="5"/>
@@ -8695,63 +8708,63 @@
         <v>142</v>
       </c>
       <c r="B157" s="16">
-        <f>SUM(B94:B124)</f>
+        <f t="shared" ref="B157:P157" si="6">SUM(B94:B124)</f>
         <v>72</v>
       </c>
       <c r="C157" s="16">
-        <f>SUM(C94:C124)</f>
+        <f t="shared" si="6"/>
         <v>1129</v>
       </c>
       <c r="D157" s="16">
-        <f>SUM(D94:D124)</f>
+        <f t="shared" si="6"/>
         <v>2287</v>
       </c>
       <c r="E157" s="16">
-        <f>SUM(E94:E124)</f>
+        <f t="shared" si="6"/>
         <v>804</v>
       </c>
       <c r="F157" s="16">
-        <f>SUM(F94:F124)</f>
+        <f t="shared" si="6"/>
         <v>13299</v>
       </c>
       <c r="G157" s="16">
-        <f>SUM(G94:G124)</f>
+        <f t="shared" si="6"/>
         <v>29072</v>
       </c>
       <c r="H157" s="16">
-        <f>SUM(H94:H124)</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="I157" s="16">
-        <f>SUM(I94:I124)</f>
+        <f t="shared" si="6"/>
         <v>2228</v>
       </c>
       <c r="J157" s="16">
-        <f>SUM(J94:J124)</f>
+        <f t="shared" si="6"/>
         <v>79358</v>
       </c>
       <c r="K157" s="16">
-        <f>SUM(K94:K124)</f>
+        <f t="shared" si="6"/>
         <v>86</v>
       </c>
       <c r="L157" s="16">
-        <f>SUM(L94:L124)</f>
+        <f t="shared" si="6"/>
         <v>1386</v>
       </c>
       <c r="M157" s="16">
-        <f>SUM(M94:M124)</f>
+        <f t="shared" si="6"/>
         <v>35820</v>
       </c>
       <c r="N157" s="16">
-        <f>SUM(N94:N124)</f>
+        <f t="shared" si="6"/>
         <v>1320</v>
       </c>
       <c r="O157" s="16">
-        <f>SUM(O94:O124)</f>
+        <f t="shared" si="6"/>
         <v>1321</v>
       </c>
       <c r="P157" s="16">
-        <f>SUM(P94:P124)</f>
+        <f t="shared" si="6"/>
         <v>168198</v>
       </c>
       <c r="Q157" s="5"/>
@@ -8765,59 +8778,59 @@
         <v>130</v>
       </c>
       <c r="C158" s="16">
-        <f t="shared" ref="C158:P158" si="4">SUM(C126:C148)</f>
+        <f t="shared" ref="C158:P158" si="7">SUM(C126:C148)</f>
         <v>41</v>
       </c>
       <c r="D158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="E158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="F158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1766</v>
       </c>
       <c r="G158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1180</v>
       </c>
       <c r="H158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>339</v>
       </c>
       <c r="I158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>776</v>
       </c>
       <c r="J158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1599</v>
       </c>
       <c r="K158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="L158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>237</v>
       </c>
       <c r="M158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4999</v>
       </c>
       <c r="N158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1145</v>
       </c>
       <c r="O158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9865</v>
       </c>
       <c r="P158" s="16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>22154</v>
       </c>
       <c r="Q158" s="5"/>
@@ -8831,64 +8844,64 @@
         <v>120</v>
       </c>
       <c r="C159" s="16">
-        <f t="shared" ref="C159:P159" si="5">SUM(C150:C153)</f>
+        <f t="shared" ref="C159:P159" si="8">SUM(C150:C153)</f>
         <v>623</v>
       </c>
       <c r="D159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>103</v>
       </c>
       <c r="E159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>97</v>
       </c>
       <c r="F159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>56</v>
       </c>
       <c r="G159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="H159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>117</v>
       </c>
       <c r="I159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>167</v>
       </c>
       <c r="J159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>589</v>
       </c>
       <c r="K159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>49</v>
       </c>
       <c r="M159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>11683</v>
       </c>
       <c r="N159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6503</v>
       </c>
       <c r="O159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>12768</v>
       </c>
       <c r="P159" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>32897</v>
       </c>
       <c r="Q159" s="5"/>
     </row>
-    <row r="160" spans="1:17" s="7" customFormat="1" ht="12.2" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:17" s="7" customFormat="1" ht="12.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A160" s="8" t="s">
         <v>145</v>
       </c>
@@ -8897,64 +8910,64 @@
         <v>91405</v>
       </c>
       <c r="C160" s="9">
-        <f t="shared" ref="C160:P160" si="6">SUM(C155:C159)</f>
+        <f t="shared" ref="C160:P160" si="9">SUM(C155:C159)</f>
         <v>37775</v>
       </c>
       <c r="D160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>120449</v>
       </c>
       <c r="E160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>154228</v>
       </c>
       <c r="F160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>128118</v>
       </c>
       <c r="G160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>55415</v>
       </c>
       <c r="H160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4605</v>
       </c>
       <c r="I160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10411</v>
       </c>
       <c r="J160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>532002</v>
       </c>
       <c r="K160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1694</v>
       </c>
       <c r="L160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>72539</v>
       </c>
       <c r="M160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>171889</v>
       </c>
       <c r="N160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17117</v>
       </c>
       <c r="O160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>32507</v>
       </c>
       <c r="P160" s="9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>1430154</v>
       </c>
       <c r="Q160" s="14"/>
     </row>
-    <row r="161" spans="17:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="17:17" x14ac:dyDescent="0.2">
       <c r="Q161" s="15"/>
     </row>
   </sheetData>

</xml_diff>